<commit_message>
General updates to include BC and OC scaling. 1. Update Japan and REAS inventories to include OC and BC. 2. Use SPEW EFs all the way bac to 1960 (previously, 1964 value written to 1960-1964 and caused spike in jpn) 3. Bug fix in scaling_emission_functions to account for scaling inventories where the min_inventory_year is not a later year than the first non-NaN year in the regional inventory data. (i.e. min year set to 1980 but first non-NaN year is 1985). This case would previously cause a fatal error.
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/REAS_scaling_mapping.xlsx
+++ b/input/mappings/scaling/REAS_scaling_mapping.xlsx
@@ -1,18 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emcduffie/Documents/GEOS-Chem/CEDS/CEDS_v0611/input/mappings/scaling/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D06A43D0-8E75-9B4C-940D-FFB039EA873D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17500" yWindow="3540" windowWidth="24120" windowHeight="13620" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="14280" yWindow="3540" windowWidth="24120" windowHeight="13620" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
     <sheet name="method" sheetId="2" r:id="rId2"/>
     <sheet name="year" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -21,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="203">
   <si>
     <t>pre_ext_method</t>
   </si>
@@ -618,12 +630,24 @@
   </si>
   <si>
     <t>1A3dii_Domestic-navigation</t>
+  </si>
+  <si>
+    <t>Big jump in road emissions after 2008</t>
+  </si>
+  <si>
+    <t>afg</t>
+  </si>
+  <si>
+    <t>khm</t>
+  </si>
+  <si>
+    <t>Doubling of residential emissions between 2008 and 2009</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -673,6 +697,7 @@
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1933,29 +1958,29 @@
   </cellXfs>
   <cellStyles count="725">
     <cellStyle name="20% - Accent1" xfId="580" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent1 2" xfId="607"/>
+    <cellStyle name="20% - Accent1 2" xfId="607" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="20% - Accent2" xfId="584" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2 2" xfId="609"/>
+    <cellStyle name="20% - Accent2 2" xfId="609" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="20% - Accent3" xfId="588" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3 2" xfId="611"/>
+    <cellStyle name="20% - Accent3 2" xfId="611" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="20% - Accent4" xfId="592" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4 2" xfId="613"/>
+    <cellStyle name="20% - Accent4 2" xfId="613" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="20% - Accent5" xfId="596" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5 2" xfId="615"/>
+    <cellStyle name="20% - Accent5 2" xfId="615" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="20% - Accent6" xfId="600" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6 2" xfId="617"/>
+    <cellStyle name="20% - Accent6 2" xfId="617" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="40% - Accent1" xfId="581" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1 2" xfId="608"/>
+    <cellStyle name="40% - Accent1 2" xfId="608" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
     <cellStyle name="40% - Accent2" xfId="585" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2 2" xfId="610"/>
+    <cellStyle name="40% - Accent2 2" xfId="610" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
     <cellStyle name="40% - Accent3" xfId="589" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3 2" xfId="612"/>
+    <cellStyle name="40% - Accent3 2" xfId="612" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="40% - Accent4" xfId="593" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4 2" xfId="614"/>
+    <cellStyle name="40% - Accent4 2" xfId="614" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
     <cellStyle name="40% - Accent5" xfId="597" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5 2" xfId="616"/>
+    <cellStyle name="40% - Accent5 2" xfId="616" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
     <cellStyle name="40% - Accent6" xfId="601" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6 2" xfId="618"/>
+    <cellStyle name="40% - Accent6 2" xfId="618" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
     <cellStyle name="60% - Accent1" xfId="582" builtinId="32" customBuiltin="1"/>
     <cellStyle name="60% - Accent2" xfId="586" builtinId="36" customBuiltin="1"/>
     <cellStyle name="60% - Accent3" xfId="590" builtinId="40" customBuiltin="1"/>
@@ -2649,10 +2674,10 @@
     <cellStyle name="Linked Cell" xfId="574" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="570" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="603"/>
-    <cellStyle name="Normal 3" xfId="605"/>
-    <cellStyle name="Note 2" xfId="604"/>
-    <cellStyle name="Note 3" xfId="606"/>
+    <cellStyle name="Normal 2" xfId="603" xr:uid="{00000000-0005-0000-0000-0000CD020000}"/>
+    <cellStyle name="Normal 3" xfId="605" xr:uid="{00000000-0005-0000-0000-0000CE020000}"/>
+    <cellStyle name="Note 2" xfId="604" xr:uid="{00000000-0005-0000-0000-0000CF020000}"/>
+    <cellStyle name="Note 3" xfId="606" xr:uid="{00000000-0005-0000-0000-0000D0020000}"/>
     <cellStyle name="Output" xfId="572" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="563" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="578" builtinId="25" customBuiltin="1"/>
@@ -2663,6 +2688,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2989,17 +3017,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C37" sqref="C37"/>
+      <selection pane="bottomRight" activeCell="A29" sqref="A29:XFD35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.83203125" customWidth="1"/>
     <col min="2" max="2" width="27.1640625" customWidth="1"/>
@@ -3008,7 +3036,7 @@
     <col min="7" max="7" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -3022,7 +3050,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>81</v>
       </c>
@@ -3033,7 +3061,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>80</v>
       </c>
@@ -3044,7 +3072,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>86</v>
       </c>
@@ -3055,7 +3083,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>87</v>
       </c>
@@ -3063,7 +3091,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>88</v>
       </c>
@@ -3071,7 +3099,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="93" t="s">
         <v>190</v>
       </c>
@@ -3079,10 +3107,10 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="93"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>62</v>
       </c>
@@ -3090,7 +3118,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>82</v>
       </c>
@@ -3101,7 +3129,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>83</v>
       </c>
@@ -3112,7 +3140,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>84</v>
       </c>
@@ -3123,7 +3151,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>62</v>
       </c>
@@ -3131,7 +3159,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>62</v>
       </c>
@@ -3139,7 +3167,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>85</v>
       </c>
@@ -3150,7 +3178,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>62</v>
       </c>
@@ -3158,7 +3186,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>62</v>
       </c>
@@ -3166,7 +3194,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>62</v>
       </c>
@@ -3174,7 +3202,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>62</v>
       </c>
@@ -3182,7 +3210,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>62</v>
       </c>
@@ -3190,7 +3218,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>62</v>
       </c>
@@ -3198,7 +3226,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
         <v>89</v>
       </c>
@@ -3209,7 +3237,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
         <v>90</v>
       </c>
@@ -3217,7 +3245,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
         <v>91</v>
       </c>
@@ -3225,7 +3253,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
         <v>92</v>
       </c>
@@ -3233,7 +3261,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="93" t="s">
         <v>182</v>
       </c>
@@ -3244,11 +3272,11 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="93"/>
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
         <v>93</v>
       </c>
@@ -3256,7 +3284,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="19" t="s">
         <v>95</v>
       </c>
@@ -3264,7 +3292,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="18" t="s">
         <v>94</v>
       </c>
@@ -3272,7 +3300,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="21" t="s">
         <v>97</v>
       </c>
@@ -3280,7 +3308,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="20" t="s">
         <v>96</v>
       </c>
@@ -3288,7 +3316,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="22" t="s">
         <v>98</v>
       </c>
@@ -3296,7 +3324,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="23" t="s">
         <v>99</v>
       </c>
@@ -3307,7 +3335,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="24" t="s">
         <v>100</v>
       </c>
@@ -3318,7 +3346,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="25" t="s">
         <v>101</v>
       </c>
@@ -3326,7 +3354,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>64</v>
       </c>
@@ -3334,7 +3362,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="26" t="s">
         <v>102</v>
       </c>
@@ -3345,7 +3373,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="27" t="s">
         <v>103</v>
       </c>
@@ -3356,7 +3384,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="28" t="s">
         <v>104</v>
       </c>
@@ -3367,7 +3395,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="29" t="s">
         <v>105</v>
       </c>
@@ -3375,7 +3403,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="30" t="s">
         <v>106</v>
       </c>
@@ -3383,7 +3411,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="79" t="s">
         <v>156</v>
       </c>
@@ -3391,7 +3419,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="93" t="s">
         <v>181</v>
       </c>
@@ -3399,7 +3427,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="31" t="s">
         <v>107</v>
       </c>
@@ -3411,7 +3439,7 @@
       </c>
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="33" t="s">
         <v>109</v>
       </c>
@@ -3423,7 +3451,7 @@
       </c>
       <c r="D49" s="3"/>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="32" t="s">
         <v>108</v>
       </c>
@@ -3432,7 +3460,7 @@
       </c>
       <c r="D50" s="3"/>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="34" t="s">
         <v>110</v>
       </c>
@@ -3440,7 +3468,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="36" t="s">
         <v>112</v>
       </c>
@@ -3449,7 +3477,7 @@
       </c>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="77" t="s">
         <v>154</v>
       </c>
@@ -3458,7 +3486,7 @@
       </c>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="78" t="s">
         <v>155</v>
       </c>
@@ -3467,7 +3495,7 @@
       </c>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="93" t="s">
         <v>183</v>
       </c>
@@ -3478,7 +3506,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="35" t="s">
         <v>111</v>
       </c>
@@ -3486,7 +3514,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="42" t="s">
         <v>118</v>
       </c>
@@ -3494,7 +3522,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="45" t="s">
         <v>121</v>
       </c>
@@ -3502,7 +3530,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="44" t="s">
         <v>120</v>
       </c>
@@ -3513,7 +3541,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="83" t="s">
         <v>130</v>
       </c>
@@ -3521,7 +3549,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="43" t="s">
         <v>119</v>
       </c>
@@ -3529,7 +3557,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="41" t="s">
         <v>117</v>
       </c>
@@ -3540,7 +3568,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>66</v>
       </c>
@@ -3548,7 +3576,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="93" t="s">
         <v>186</v>
       </c>
@@ -3556,7 +3584,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="93" t="s">
         <v>187</v>
       </c>
@@ -3564,7 +3592,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="46" t="s">
         <v>122</v>
       </c>
@@ -3575,7 +3603,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="47" t="s">
         <v>123</v>
       </c>
@@ -3583,7 +3611,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="38" t="s">
         <v>114</v>
       </c>
@@ -3591,7 +3619,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="37" t="s">
         <v>113</v>
       </c>
@@ -3599,7 +3627,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="48" t="s">
         <v>124</v>
       </c>
@@ -3607,7 +3635,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="49" t="s">
         <v>125</v>
       </c>
@@ -3615,7 +3643,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="50" t="s">
         <v>126</v>
       </c>
@@ -3623,7 +3651,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="39" t="s">
         <v>115</v>
       </c>
@@ -3631,7 +3659,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="51" t="s">
         <v>127</v>
       </c>
@@ -3639,7 +3667,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="86" t="s">
         <v>168</v>
       </c>
@@ -3647,7 +3675,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="52" t="s">
         <v>128</v>
       </c>
@@ -3658,7 +3686,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="53" t="s">
         <v>129</v>
       </c>
@@ -3666,7 +3694,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="54" t="s">
         <v>131</v>
       </c>
@@ -3674,7 +3702,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="55" t="s">
         <v>132</v>
       </c>
@@ -3685,7 +3713,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="56" t="s">
         <v>133</v>
       </c>
@@ -3693,7 +3721,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="40" t="s">
         <v>116</v>
       </c>
@@ -3701,7 +3729,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="57" t="s">
         <v>134</v>
       </c>
@@ -3709,7 +3737,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="58" t="s">
         <v>135</v>
       </c>
@@ -3717,30 +3745,30 @@
         <v>71</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="2"/>
       <c r="B86" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="2"/>
       <c r="B87" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="2"/>
       <c r="B88" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="59" t="s">
         <v>136</v>
       </c>
@@ -3748,7 +3776,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="60" t="s">
         <v>137</v>
       </c>
@@ -3756,7 +3784,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="61" t="s">
         <v>138</v>
       </c>
@@ -3764,7 +3792,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="62" t="s">
         <v>139</v>
       </c>
@@ -3772,7 +3800,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="75" t="s">
         <v>152</v>
       </c>
@@ -3780,7 +3808,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="76" t="s">
         <v>153</v>
       </c>
@@ -3788,7 +3816,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="84" t="s">
         <v>166</v>
       </c>
@@ -3796,7 +3824,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="88" t="s">
         <v>173</v>
       </c>
@@ -3804,7 +3832,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="89" t="s">
         <v>174</v>
       </c>
@@ -3812,7 +3840,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="90" t="s">
         <v>175</v>
       </c>
@@ -3820,7 +3848,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="90" t="s">
         <v>176</v>
       </c>
@@ -3828,7 +3856,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="63" t="s">
         <v>140</v>
       </c>
@@ -3839,7 +3867,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="64" t="s">
         <v>141</v>
       </c>
@@ -3850,7 +3878,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="65" t="s">
         <v>142</v>
       </c>
@@ -3861,7 +3889,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="66" t="s">
         <v>143</v>
       </c>
@@ -3872,7 +3900,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="67" t="s">
         <v>144</v>
       </c>
@@ -3880,7 +3908,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="85" t="s">
         <v>167</v>
       </c>
@@ -3888,7 +3916,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="91" t="s">
         <v>177</v>
       </c>
@@ -3896,7 +3924,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="91" t="s">
         <v>178</v>
       </c>
@@ -3904,7 +3932,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="94" t="s">
         <v>77</v>
       </c>
@@ -3912,7 +3940,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="68" t="s">
         <v>145</v>
       </c>
@@ -3923,7 +3951,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="69" t="s">
         <v>146</v>
       </c>
@@ -3934,7 +3962,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="70" t="s">
         <v>147</v>
       </c>
@@ -3942,7 +3970,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="71" t="s">
         <v>148</v>
       </c>
@@ -3953,7 +3981,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="72" t="s">
         <v>149</v>
       </c>
@@ -3961,7 +3989,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="73" t="s">
         <v>150</v>
       </c>
@@ -3969,7 +3997,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="74" t="s">
         <v>151</v>
       </c>
@@ -3977,28 +4005,28 @@
         <v>78</v>
       </c>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="2"/>
       <c r="C120" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C121" t="s">
         <v>30</v>
       </c>
       <c r="D121" s="3"/>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C122" t="s">
         <v>21</v>
       </c>
       <c r="D122" s="3"/>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D123" s="3"/>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="82" t="s">
         <v>157</v>
       </c>
@@ -4009,7 +4037,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="82" t="s">
         <v>159</v>
       </c>
@@ -4017,7 +4045,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" s="82" t="s">
         <v>161</v>
       </c>
@@ -4028,7 +4056,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" s="82" t="s">
         <v>158</v>
       </c>
@@ -4036,7 +4064,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="82" t="s">
         <v>162</v>
       </c>
@@ -4044,7 +4072,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="129" spans="1:3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" s="82" t="s">
         <v>165</v>
       </c>
@@ -4052,7 +4080,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="130" spans="1:3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" s="82" t="s">
         <v>164</v>
       </c>
@@ -4063,7 +4091,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="131" spans="1:3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" s="82" t="s">
         <v>160</v>
       </c>
@@ -4071,7 +4099,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="132" spans="1:3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="87" t="s">
         <v>169</v>
       </c>
@@ -4082,7 +4110,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="133" spans="1:3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="87" t="s">
         <v>170</v>
       </c>
@@ -4090,7 +4118,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="134" spans="1:3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="87" t="s">
         <v>171</v>
       </c>
@@ -4098,7 +4126,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="135" spans="1:3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="87" t="s">
         <v>172</v>
       </c>
@@ -4106,7 +4134,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="136" spans="1:3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="82" t="s">
         <v>163</v>
       </c>
@@ -4114,7 +4142,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="138" spans="1:3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="80" t="s">
         <v>179</v>
       </c>
@@ -4125,7 +4153,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="139" spans="1:3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" s="92" t="s">
         <v>180</v>
       </c>
@@ -4133,7 +4161,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="141" spans="1:3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" s="93" t="s">
         <v>184</v>
       </c>
@@ -4141,7 +4169,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="142" spans="1:3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" s="93" t="s">
         <v>185</v>
       </c>
@@ -4149,7 +4177,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="144" spans="1:3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" s="93" t="s">
         <v>188</v>
       </c>
@@ -4157,7 +4185,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="145" spans="1:2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" s="93" t="s">
         <v>189</v>
       </c>
@@ -4166,7 +4194,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:C84">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C84">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4180,21 +4208,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="15.83203125" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -4211,7 +4239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -4240,19 +4268,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -4278,7 +4306,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -4299,6 +4327,58 @@
       </c>
       <c r="G2" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3">
+        <v>1960</v>
+      </c>
+      <c r="D3">
+        <v>2008</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3">
+        <v>2000</v>
+      </c>
+      <c r="G3">
+        <v>2008</v>
+      </c>
+      <c r="H3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4">
+        <v>1960</v>
+      </c>
+      <c r="D4">
+        <v>2008</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4">
+        <v>2000</v>
+      </c>
+      <c r="G4">
+        <v>2008</v>
+      </c>
+      <c r="H4" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>